<commit_message>
rms aula03 correcores requisitos
</commit_message>
<xml_diff>
--- a/3des/chamada.xlsx
+++ b/3des/chamada.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wellington\senai2023\3des\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\senai2023\3des\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3715393D-E5EC-44D1-8F68-4733D0ED1665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A6829C-B5AB-4842-8BEB-025DEBA452BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chamada" sheetId="5" r:id="rId1"/>
@@ -28,12 +28,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -41,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="56">
   <si>
     <t>Aluno</t>
   </si>
@@ -686,9 +683,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE8BBDE-6D60-438E-A327-880B06C9683B}">
   <dimension ref="A1:AK29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AB29" sqref="AB29"/>
+      <selection pane="topRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3734,8 +3731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE0EAD6-6256-40A7-B315-10C2E7E1019B}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3780,26 +3777,41 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="E7">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -3813,64 +3825,97 @@
       <c r="A10" t="s">
         <v>8</v>
       </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
+      <c r="E12">
+        <v>8</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
+      <c r="E14">
+        <v>8</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
+      <c r="E15">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="E16">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
+      <c r="E18">
+        <v>9</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
+      <c r="E19">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
+      <c r="E20">
+        <v>8</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
+      <c r="E21">
+        <v>10</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -3884,33 +3929,48 @@
       <c r="A23" t="s">
         <v>21</v>
       </c>
+      <c r="E23">
+        <v>7</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
+      <c r="E24">
+        <v>8</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
+      <c r="E25">
+        <v>10</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="E26">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
+      <c r="E27">
+        <v>8</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
+      </c>
+      <c r="E28">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -3929,7 +3989,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B6" sqref="B6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4102,7 +4162,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:D13"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4184,9 +4244,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>50</v>
-      </c>
+      <c r="A9" s="3"/>
       <c r="C9" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
conteudos 3des e excel
</commit_message>
<xml_diff>
--- a/3des/chamada.xlsx
+++ b/3des/chamada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wellington\senai2023\3des\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D569C7F-2477-414A-BC74-A7BBFC324C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB87FB4-C9CA-45E0-AD4B-290F25FFB614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="56">
   <si>
     <t>Aluno</t>
   </si>
@@ -708,7 +708,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AE1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AL23" sqref="AL23"/>
+      <selection pane="topRight" activeCell="AM1" sqref="AM1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1187,6 +1187,9 @@
       <c r="AL3" s="7" t="s">
         <v>36</v>
       </c>
+      <c r="AM3" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="4" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1303,6 +1306,9 @@
       <c r="AL4" s="7" t="s">
         <v>37</v>
       </c>
+      <c r="AM4" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1419,6 +1425,9 @@
       <c r="AL5" s="7" t="s">
         <v>37</v>
       </c>
+      <c r="AM5" s="7" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="6" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1535,6 +1544,9 @@
       <c r="AL6" s="7" t="s">
         <v>36</v>
       </c>
+      <c r="AM6" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="7" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1651,6 +1663,9 @@
       <c r="AL7" s="7" t="s">
         <v>37</v>
       </c>
+      <c r="AM7" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="8" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1767,6 +1782,9 @@
       <c r="AL8" s="7" t="s">
         <v>36</v>
       </c>
+      <c r="AM8" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="9" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1883,6 +1901,9 @@
       <c r="AL9" s="7" t="s">
         <v>36</v>
       </c>
+      <c r="AM9" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="10" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1999,6 +2020,9 @@
       <c r="AL10" s="7" t="s">
         <v>36</v>
       </c>
+      <c r="AM10" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="11" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -2115,6 +2139,9 @@
       <c r="AL11" s="7" t="s">
         <v>36</v>
       </c>
+      <c r="AM11" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="12" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -2231,6 +2258,9 @@
       <c r="AL12" s="7" t="s">
         <v>36</v>
       </c>
+      <c r="AM12" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="13" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -2347,6 +2377,9 @@
       <c r="AL13" s="7" t="s">
         <v>36</v>
       </c>
+      <c r="AM13" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="14" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -2463,6 +2496,9 @@
       <c r="AL14" s="7" t="s">
         <v>36</v>
       </c>
+      <c r="AM14" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -2579,6 +2615,9 @@
       <c r="AL15" s="7" t="s">
         <v>36</v>
       </c>
+      <c r="AM15" s="7" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="16" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -2695,8 +2734,11 @@
       <c r="AL16" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM16" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -2811,8 +2853,11 @@
       <c r="AL17" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM17" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -2927,8 +2972,11 @@
       <c r="AL18" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM18" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -3043,8 +3091,11 @@
       <c r="AL19" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM19" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -3159,8 +3210,11 @@
       <c r="AL20" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM20" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -3275,8 +3329,11 @@
       <c r="AL21" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM21" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -3391,8 +3448,11 @@
       <c r="AL22" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM22" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -3507,8 +3567,11 @@
       <c r="AL23" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM23" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -3623,8 +3686,11 @@
       <c r="AL24" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM24" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -3739,8 +3805,11 @@
       <c r="AL25" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM25" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -3855,8 +3924,11 @@
       <c r="AL26" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM26" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -3971,8 +4043,11 @@
       <c r="AL27" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM27" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -4087,8 +4162,11 @@
       <c r="AL28" s="7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM28" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -4201,6 +4279,9 @@
         <v>36</v>
       </c>
       <c r="AL29" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM29" s="7" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>